<commit_message>
feat: ver1, doc upload
</commit_message>
<xml_diff>
--- a/Fill-in/testFile.xlsx
+++ b/Fill-in/testFile.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yenkuangchen/Projects/NTU-hospital-automatic-support/Fill-in/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13AB0842-53FB-0B45-9759-6BAE25C5F1BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34560" yWindow="500" windowWidth="51200" windowHeight="28300"/>
+    <workbookView xWindow="34560" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="謝醫師想匯入之資料" sheetId="1" r:id="rId1"/>
     <sheet name="對比用資料" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="false"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="272">
   <si>
     <t>4229-LiSC-0904</t>
   </si>
@@ -538,11 +539,11 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <charset val="136"/>
-        <family val="2"/>
-        <color theme="1"/>
-        <sz val="12"/>
         <scheme val="minor"/>
       </rPr>
       <t>hMJ</t>
@@ -731,11 +732,11 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <charset val="136"/>
-        <family val="2"/>
-        <color theme="1"/>
-        <sz val="12"/>
         <scheme val="minor"/>
       </rPr>
       <t>andness</t>
@@ -932,236 +933,11 @@
     <t>name</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
-  <si>
-    <t>07-14-16</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>16.8416666666667</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>01-20-14</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>24.3055555555556</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>10-09-08</t>
-  </si>
-  <si>
-    <t>36.1611111111111</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>10-08-15</t>
-  </si>
-  <si>
-    <t>25.6888888888889</t>
-  </si>
-  <si>
-    <t>10-24-11</t>
-  </si>
-  <si>
-    <t>36.3444444444444</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>0.15</t>
-  </si>
-  <si>
-    <t>10-13-10</t>
-  </si>
-  <si>
-    <t>22.2555555555556</t>
-  </si>
-  <si>
-    <t>09-05-08</t>
-  </si>
-  <si>
-    <t>36.6916666666667</t>
-  </si>
-  <si>
-    <t>06-23-15</t>
-  </si>
-  <si>
-    <t>19.1805555555556</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>08-17-11</t>
-  </si>
-  <si>
-    <t>24.5583333333333</t>
-  </si>
-  <si>
-    <t>05-29-12</t>
-  </si>
-  <si>
-    <t>34.6444444444444</t>
-  </si>
-  <si>
-    <t>02-05-16</t>
-  </si>
-  <si>
-    <t>33.7638888888889</t>
-  </si>
-  <si>
-    <t>07-01-14</t>
-  </si>
-  <si>
-    <t>28.2472222222222</t>
-  </si>
-  <si>
-    <t>11-12-08</t>
-  </si>
-  <si>
-    <t>17.7555555555556</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>0.5</t>
-  </si>
-  <si>
-    <t>09-11-08</t>
-  </si>
-  <si>
-    <t>23.975</t>
-  </si>
-  <si>
-    <t>0.333</t>
-  </si>
-  <si>
-    <t>03-28-11</t>
-  </si>
-  <si>
-    <t>22.2388888888889</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>11-10-11</t>
-  </si>
-  <si>
-    <t>27.0416666666667</t>
-  </si>
-  <si>
-    <t>07-26-12</t>
-  </si>
-  <si>
-    <t>28.1111111111111</t>
-  </si>
-  <si>
-    <t>12-07-15</t>
-  </si>
-  <si>
-    <t>23.1944444444444</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>11-08-12</t>
-  </si>
-  <si>
-    <t>27.4</t>
-  </si>
-  <si>
-    <t>11-25-11</t>
-  </si>
-  <si>
-    <t>25.3944444444444</t>
-  </si>
-  <si>
-    <t>02-23-12</t>
-  </si>
-  <si>
-    <t>24.5277777777778</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>09-04-08</t>
-  </si>
-  <si>
-    <t>42.2694444444444</t>
-  </si>
-  <si>
-    <t>10-05-11</t>
-  </si>
-  <si>
-    <t>18.8111111111111</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>09-12-12</t>
-  </si>
-  <si>
-    <t>22.2833333333333</t>
-  </si>
-  <si>
-    <t>03-24-10</t>
-  </si>
-  <si>
-    <t>17.2222222222222</t>
-  </si>
-  <si>
-    <t>10-21-08</t>
-  </si>
-  <si>
-    <t>32.9555555555556</t>
-  </si>
-  <si>
-    <t>1.5</t>
-  </si>
-  <si>
-    <t>11-16-15</t>
-  </si>
-  <si>
-    <t>21.3138888888889</t>
-  </si>
-  <si>
-    <t>08-12-10</t>
-  </si>
-  <si>
-    <t>20.4861111111111</t>
-  </si>
-  <si>
-    <t>04-02-12</t>
-  </si>
-  <si>
-    <t>28.9138888888889</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00_ "/>
   </numFmts>
@@ -1242,55 +1018,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyAlignment="true">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFill="true" applyAlignment="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFill="true" applyAlignment="true">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyAlignment="true">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyAlignment="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyAlignment="true">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFill="true" applyAlignment="true">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyAlignment="true">
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyAlignment="true">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyFill="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1298,7 +1074,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1633,13 +1409,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H32" sqref="B2:H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
-    <col customWidth="true" max="1" min="1" style="2" width="24.83203125"/>
+    <col min="1" max="1" width="24.83203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -1673,547 +1449,106 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>148</v>
-      </c>
-      <c r="C2" t="s">
-        <v>209</v>
-      </c>
-      <c r="D2" t="s">
-        <v>329</v>
-      </c>
-      <c r="E2" t="s">
-        <v>273</v>
-      </c>
-      <c r="F2" t="s">
-        <v>330</v>
-      </c>
-      <c r="G2" t="s">
-        <v>288</v>
-      </c>
-      <c r="H2" t="s">
-        <v>276</v>
-      </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>149</v>
-      </c>
-      <c r="C3" t="s">
-        <v>210</v>
-      </c>
-      <c r="D3" t="s">
-        <v>292</v>
-      </c>
-      <c r="E3" t="s">
-        <v>273</v>
-      </c>
-      <c r="F3" t="s">
-        <v>293</v>
-      </c>
-      <c r="G3" t="s">
-        <v>288</v>
-      </c>
-      <c r="H3" t="s">
-        <v>276</v>
-      </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>150</v>
-      </c>
-      <c r="C4" t="s">
-        <v>211</v>
-      </c>
-      <c r="D4" t="s">
-        <v>309</v>
-      </c>
-      <c r="E4" t="s">
-        <v>278</v>
-      </c>
-      <c r="F4" t="s">
-        <v>310</v>
-      </c>
-      <c r="G4" t="s">
-        <v>280</v>
-      </c>
-      <c r="H4" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>151</v>
-      </c>
-      <c r="C5" t="s">
-        <v>212</v>
-      </c>
-      <c r="D5" t="s">
-        <v>281</v>
-      </c>
-      <c r="E5" t="s">
-        <v>273</v>
-      </c>
-      <c r="F5" t="s">
-        <v>282</v>
-      </c>
-      <c r="G5" t="s">
-        <v>283</v>
-      </c>
-      <c r="H5" t="s">
-        <v>276</v>
-      </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
-        <v>152</v>
-      </c>
-      <c r="C6" t="s">
-        <v>213</v>
-      </c>
-      <c r="D6" t="s">
-        <v>338</v>
-      </c>
-      <c r="E6" t="s">
-        <v>278</v>
-      </c>
-      <c r="F6" t="s">
-        <v>339</v>
-      </c>
-      <c r="G6" t="s">
-        <v>288</v>
-      </c>
-      <c r="H6" t="s">
-        <v>340</v>
-      </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
-        <v>153</v>
-      </c>
-      <c r="C7" t="s">
-        <v>214</v>
-      </c>
-      <c r="D7" t="s">
-        <v>305</v>
-      </c>
-      <c r="E7" t="s">
-        <v>278</v>
-      </c>
-      <c r="F7" t="s">
-        <v>306</v>
-      </c>
-      <c r="G7" t="s">
-        <v>307</v>
-      </c>
-      <c r="H7" t="s">
-        <v>308</v>
-      </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
-        <v>168</v>
-      </c>
-      <c r="C8" t="s">
-        <v>228</v>
-      </c>
-      <c r="D8" t="s">
-        <v>336</v>
-      </c>
-      <c r="E8" t="s">
-        <v>278</v>
-      </c>
-      <c r="F8" t="s">
-        <v>337</v>
-      </c>
-      <c r="G8" t="s">
-        <v>307</v>
-      </c>
-      <c r="H8" t="s">
-        <v>276</v>
-      </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
-        <v>173</v>
-      </c>
-      <c r="C9" t="s">
-        <v>233</v>
-      </c>
-      <c r="D9" t="s">
-        <v>343</v>
-      </c>
-      <c r="E9" t="s">
-        <v>273</v>
-      </c>
-      <c r="F9" t="s">
-        <v>344</v>
-      </c>
-      <c r="G9" t="s">
-        <v>314</v>
-      </c>
-      <c r="H9" t="s">
-        <v>276</v>
-      </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
-        <v>174</v>
-      </c>
-      <c r="C10" t="s">
-        <v>234</v>
-      </c>
-      <c r="D10" t="s">
-        <v>290</v>
-      </c>
-      <c r="E10" t="s">
-        <v>278</v>
-      </c>
-      <c r="F10" t="s">
-        <v>291</v>
-      </c>
-      <c r="G10" t="s">
-        <v>280</v>
-      </c>
-      <c r="H10" t="s">
-        <v>276</v>
-      </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
-        <v>176</v>
-      </c>
-      <c r="C11" t="s">
-        <v>236</v>
-      </c>
-      <c r="D11" t="s">
-        <v>312</v>
-      </c>
-      <c r="E11" t="s">
-        <v>273</v>
-      </c>
-      <c r="F11" t="s">
-        <v>313</v>
-      </c>
-      <c r="G11" t="s">
-        <v>314</v>
-      </c>
-      <c r="H11" t="s">
-        <v>276</v>
-      </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
-        <v>177</v>
-      </c>
-      <c r="C12" t="s">
-        <v>237</v>
-      </c>
-      <c r="D12" t="s">
-        <v>297</v>
-      </c>
-      <c r="E12" t="s">
-        <v>278</v>
-      </c>
-      <c r="F12" t="s">
-        <v>298</v>
-      </c>
-      <c r="G12" t="s">
-        <v>296</v>
-      </c>
-      <c r="H12" t="s">
-        <v>276</v>
-      </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
-        <v>178</v>
-      </c>
-      <c r="C13" t="s">
-        <v>238</v>
-      </c>
-      <c r="D13" t="s">
-        <v>331</v>
-      </c>
-      <c r="E13" t="s">
-        <v>278</v>
-      </c>
-      <c r="F13" t="s">
-        <v>332</v>
-      </c>
-      <c r="G13" t="s">
-        <v>333</v>
-      </c>
-      <c r="H13" t="s">
-        <v>276</v>
-      </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B14" t="s">
-        <v>179</v>
-      </c>
-      <c r="C14" t="s">
-        <v>239</v>
-      </c>
-      <c r="D14" t="s">
-        <v>286</v>
-      </c>
-      <c r="E14" t="s">
-        <v>278</v>
-      </c>
-      <c r="F14" t="s">
-        <v>287</v>
-      </c>
-      <c r="G14" t="s">
-        <v>288</v>
-      </c>
-      <c r="H14" t="s">
-        <v>289</v>
-      </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B15" t="s">
-        <v>180</v>
-      </c>
-      <c r="C15" t="s">
-        <v>240</v>
-      </c>
-      <c r="D15" t="s">
-        <v>315</v>
-      </c>
-      <c r="E15" t="s">
-        <v>278</v>
-      </c>
-      <c r="F15" t="s">
-        <v>316</v>
-      </c>
-      <c r="G15" t="s">
-        <v>280</v>
-      </c>
-      <c r="H15" t="s">
-        <v>278</v>
-      </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B16" t="s">
-        <v>182</v>
-      </c>
-      <c r="C16" t="s">
-        <v>242</v>
-      </c>
-      <c r="D16" t="s">
-        <v>324</v>
-      </c>
-      <c r="E16" t="s">
-        <v>273</v>
-      </c>
-      <c r="F16" t="s">
-        <v>325</v>
-      </c>
-      <c r="G16" t="s">
-        <v>314</v>
-      </c>
-      <c r="H16" t="s">
-        <v>276</v>
-      </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B17" t="s">
-        <v>183</v>
-      </c>
-      <c r="C17" t="s">
-        <v>243</v>
-      </c>
-      <c r="D17" t="s">
-        <v>326</v>
-      </c>
-      <c r="E17" t="s">
-        <v>273</v>
-      </c>
-      <c r="F17" t="s">
-        <v>327</v>
-      </c>
-      <c r="G17" t="s">
-        <v>328</v>
-      </c>
-      <c r="H17" t="s">
-        <v>276</v>
-      </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B18" t="s">
-        <v>184</v>
-      </c>
-      <c r="C18" t="s">
-        <v>244</v>
-      </c>
-      <c r="D18" t="s">
-        <v>345</v>
-      </c>
-      <c r="E18" t="s">
-        <v>278</v>
-      </c>
-      <c r="F18" t="s">
-        <v>346</v>
-      </c>
-      <c r="G18" t="s">
-        <v>275</v>
-      </c>
-      <c r="H18" t="s">
-        <v>276</v>
-      </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B19" t="s">
-        <v>186</v>
-      </c>
-      <c r="C19" t="s">
-        <v>246</v>
-      </c>
-      <c r="D19" t="s">
-        <v>299</v>
-      </c>
-      <c r="E19" t="s">
-        <v>273</v>
-      </c>
-      <c r="F19" t="s">
-        <v>300</v>
-      </c>
-      <c r="G19" t="s">
-        <v>280</v>
-      </c>
-      <c r="H19" t="s">
-        <v>276</v>
-      </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B20" t="s">
-        <v>187</v>
-      </c>
-      <c r="C20" t="s">
-        <v>247</v>
-      </c>
-      <c r="D20" t="s">
-        <v>317</v>
-      </c>
-      <c r="E20" t="s">
-        <v>273</v>
-      </c>
-      <c r="F20" t="s">
-        <v>318</v>
-      </c>
-      <c r="G20" t="s">
-        <v>280</v>
-      </c>
-      <c r="H20" t="s">
-        <v>276</v>
-      </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B21" t="s">
-        <v>188</v>
-      </c>
-      <c r="C21" t="s">
-        <v>248</v>
-      </c>
-      <c r="D21" t="s">
-        <v>334</v>
-      </c>
-      <c r="E21" t="s">
-        <v>273</v>
-      </c>
-      <c r="F21" t="s">
-        <v>335</v>
-      </c>
-      <c r="G21" t="s">
-        <v>280</v>
-      </c>
-      <c r="H21" t="s">
-        <v>276</v>
-      </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B22" t="s">
-        <v>175</v>
-      </c>
-      <c r="C22" t="s">
-        <v>249</v>
-      </c>
-      <c r="D22" t="s">
-        <v>322</v>
-      </c>
-      <c r="E22" t="s">
-        <v>273</v>
-      </c>
-      <c r="F22" t="s">
-        <v>323</v>
-      </c>
-      <c r="G22" t="s">
-        <v>283</v>
-      </c>
-      <c r="H22" t="s">
-        <v>276</v>
-      </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="1" t="s">
@@ -2224,53 +1559,11 @@
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B24" t="s">
-        <v>192</v>
-      </c>
-      <c r="C24" t="s">
-        <v>253</v>
-      </c>
-      <c r="D24" t="s">
-        <v>277</v>
-      </c>
-      <c r="E24" t="s">
-        <v>278</v>
-      </c>
-      <c r="F24" t="s">
-        <v>279</v>
-      </c>
-      <c r="G24" t="s">
-        <v>280</v>
-      </c>
-      <c r="H24" t="s">
-        <v>276</v>
-      </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B25" t="s">
-        <v>193</v>
-      </c>
-      <c r="C25" t="s">
-        <v>254</v>
-      </c>
-      <c r="D25" t="s">
-        <v>303</v>
-      </c>
-      <c r="E25" t="s">
-        <v>273</v>
-      </c>
-      <c r="F25" t="s">
-        <v>304</v>
-      </c>
-      <c r="G25" t="s">
-        <v>283</v>
-      </c>
-      <c r="H25" t="s">
-        <v>276</v>
-      </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="1" t="s">
@@ -2281,156 +1574,30 @@
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B27" t="s">
-        <v>197</v>
-      </c>
-      <c r="C27" t="s">
-        <v>259</v>
-      </c>
-      <c r="D27" t="s">
-        <v>294</v>
-      </c>
-      <c r="E27" t="s">
-        <v>278</v>
-      </c>
-      <c r="F27" t="s">
-        <v>295</v>
-      </c>
-      <c r="G27" t="s">
-        <v>296</v>
-      </c>
-      <c r="H27" t="s">
-        <v>276</v>
-      </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B28" t="s">
-        <v>199</v>
-      </c>
-      <c r="C28" t="s">
-        <v>261</v>
-      </c>
-      <c r="D28" t="s">
-        <v>284</v>
-      </c>
-      <c r="E28" t="s">
-        <v>273</v>
-      </c>
-      <c r="F28" t="s">
-        <v>285</v>
-      </c>
-      <c r="G28" t="s">
-        <v>283</v>
-      </c>
-      <c r="H28" t="s">
-        <v>276</v>
-      </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B29" t="s">
-        <v>200</v>
-      </c>
-      <c r="C29" t="s">
-        <v>262</v>
-      </c>
-      <c r="D29" t="s">
-        <v>341</v>
-      </c>
-      <c r="E29" t="s">
-        <v>273</v>
-      </c>
-      <c r="F29" t="s">
-        <v>342</v>
-      </c>
-      <c r="G29" t="s">
-        <v>314</v>
-      </c>
-      <c r="H29" t="s">
-        <v>276</v>
-      </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B30" t="s">
-        <v>201</v>
-      </c>
-      <c r="C30" t="s">
-        <v>263</v>
-      </c>
-      <c r="D30" t="s">
-        <v>319</v>
-      </c>
-      <c r="E30" t="s">
-        <v>278</v>
-      </c>
-      <c r="F30" t="s">
-        <v>320</v>
-      </c>
-      <c r="G30" t="s">
-        <v>321</v>
-      </c>
-      <c r="H30" t="s">
-        <v>276</v>
-      </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B31" t="s">
-        <v>202</v>
-      </c>
-      <c r="C31" t="s">
-        <v>264</v>
-      </c>
-      <c r="D31" t="s">
-        <v>301</v>
-      </c>
-      <c r="E31" t="s">
-        <v>278</v>
-      </c>
-      <c r="F31" t="s">
-        <v>302</v>
-      </c>
-      <c r="G31" t="s">
-        <v>280</v>
-      </c>
-      <c r="H31" t="s">
-        <v>276</v>
-      </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="B32" t="s">
-        <v>203</v>
-      </c>
-      <c r="C32" t="s">
-        <v>265</v>
-      </c>
-      <c r="D32" t="s">
-        <v>272</v>
-      </c>
-      <c r="E32" t="s">
-        <v>273</v>
-      </c>
-      <c r="F32" t="s">
-        <v>274</v>
-      </c>
-      <c r="G32" t="s">
-        <v>275</v>
-      </c>
-      <c r="H32" t="s">
-        <v>276</v>
       </c>
     </row>
   </sheetData>
@@ -2443,8 +1610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I112"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:I1"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="A89" sqref="A89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>

</xml_diff>